<commit_message>
correct static data(add socket connect status, correct js), replace some docks(pins, TODO), correct notes, correct list of libs, correct webserver and socket
</commit_message>
<xml_diff>
--- a/docks/САУ_мГТД.xlsx
+++ b/docks/САУ_мГТД.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esppres_my_workspace\GTD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esppres_my_workspace\GTD\docks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BAA84D25-7BD7-4FE5-9D80-8F6AE4D7B3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2641AD-C322-4F67-8CDF-7C0CE18E1EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Devkit_v4_pins_v3" sheetId="1" r:id="rId1"/>
     <sheet name="PCA_CHANELS" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="10"/>
@@ -913,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -923,14 +923,10 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -939,7 +935,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -951,40 +946,31 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Accent" xfId="2"/>
-    <cellStyle name="Accent 1" xfId="3"/>
-    <cellStyle name="Accent 2" xfId="4"/>
-    <cellStyle name="Accent 3" xfId="5"/>
-    <cellStyle name="Bad" xfId="6"/>
-    <cellStyle name="cf1" xfId="7"/>
-    <cellStyle name="Error" xfId="8"/>
-    <cellStyle name="Footnote" xfId="9"/>
-    <cellStyle name="Good" xfId="10"/>
-    <cellStyle name="Heading" xfId="11"/>
-    <cellStyle name="Heading 1" xfId="12"/>
-    <cellStyle name="Heading 2" xfId="13"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
-    <cellStyle name="Neutral" xfId="15"/>
-    <cellStyle name="Note" xfId="16"/>
-    <cellStyle name="Result" xfId="17"/>
-    <cellStyle name="Status" xfId="18"/>
-    <cellStyle name="Text" xfId="19"/>
-    <cellStyle name="Untitled1" xfId="20"/>
-    <cellStyle name="Untitled2" xfId="21"/>
-    <cellStyle name="Warning" xfId="22"/>
-    <cellStyle name="Гиперссылка" xfId="1"/>
+    <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="cf1" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Error" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Footnote" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Good" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 1" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Heading 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Neutral" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Note" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Result" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Status" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Text" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Untitled1" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Untitled2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Warning" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Гиперссылка" xfId="1" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF860D"/>
-          <bgColor rgb="FFFF860D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1341,11 +1327,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1394,7 +1380,7 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="2" t="s">
         <v>116</v>
       </c>
       <c r="K1" s="2"/>
@@ -1430,7 +1416,6 @@
       <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="12"/>
       <c r="L2" s="5">
         <v>1</v>
       </c>
@@ -1465,7 +1450,6 @@
         <v>6</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="12"/>
       <c r="L3" s="5">
         <v>2</v>
       </c>
@@ -1502,7 +1486,6 @@
         <v>8</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="12"/>
       <c r="L4" s="5">
         <v>3</v>
       </c>
@@ -1539,7 +1522,6 @@
         <v>9</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="12"/>
       <c r="L5" s="5">
         <v>4</v>
       </c>
@@ -1576,7 +1558,6 @@
         <v>2</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="12"/>
       <c r="L6" s="5">
         <v>5</v>
       </c>
@@ -1613,7 +1594,6 @@
         <v>7</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="12"/>
       <c r="L7" s="5">
         <v>6</v>
       </c>
@@ -1648,7 +1628,6 @@
         <v>15</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="12"/>
       <c r="L8" s="5">
         <v>7</v>
       </c>
@@ -1681,7 +1660,6 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="12"/>
       <c r="L9" s="5">
         <v>8</v>
       </c>
@@ -1714,7 +1692,6 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="12"/>
       <c r="L10" s="5">
         <v>9</v>
       </c>
@@ -1749,7 +1726,6 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="12"/>
       <c r="L11" s="5">
         <v>10</v>
       </c>
@@ -1784,7 +1760,6 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="12"/>
       <c r="L12" s="5">
         <v>11</v>
       </c>
@@ -1819,7 +1794,6 @@
       <c r="I13" s="4">
         <v>2</v>
       </c>
-      <c r="J13" s="12"/>
       <c r="L13" s="5">
         <v>12</v>
       </c>
@@ -1854,7 +1828,6 @@
       <c r="I14" s="4">
         <v>8</v>
       </c>
-      <c r="J14" s="12"/>
       <c r="L14" s="8">
         <v>13</v>
       </c>
@@ -1885,7 +1858,6 @@
       <c r="I15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="12"/>
       <c r="L15" s="8">
         <v>14</v>
       </c>
@@ -1916,7 +1888,6 @@
       <c r="I16" s="4">
         <v>4</v>
       </c>
-      <c r="J16" s="12"/>
       <c r="L16" s="5">
         <v>15</v>
       </c>
@@ -1947,7 +1918,6 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="12"/>
       <c r="L17" s="5">
         <v>16</v>
       </c>
@@ -1974,7 +1944,6 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="12"/>
       <c r="L18" s="5">
         <v>17</v>
       </c>
@@ -2001,7 +1970,6 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="12"/>
       <c r="L19" s="5">
         <v>18</v>
       </c>
@@ -2030,7 +1998,6 @@
         <v>13</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="12"/>
       <c r="L20" s="5">
         <v>19</v>
       </c>
@@ -2059,7 +2026,6 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="12"/>
       <c r="L21" s="5">
         <v>20</v>
       </c>
@@ -2086,7 +2052,6 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="12"/>
       <c r="L22" s="5">
         <v>21</v>
       </c>
@@ -2113,7 +2078,6 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="12"/>
       <c r="L23" s="5">
         <v>22</v>
       </c>
@@ -2144,7 +2108,6 @@
       <c r="I24" s="4">
         <v>6</v>
       </c>
-      <c r="J24" s="12"/>
       <c r="L24" s="5">
         <v>23</v>
       </c>
@@ -2179,7 +2142,6 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="12"/>
       <c r="L25" s="5">
         <v>24</v>
       </c>
@@ -2216,7 +2178,6 @@
         <v>14</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="12"/>
       <c r="L26" s="5">
         <v>25</v>
       </c>
@@ -2249,7 +2210,6 @@
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="12"/>
       <c r="L27" s="5">
         <v>26</v>
       </c>
@@ -2284,7 +2244,6 @@
         <v>3</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="12"/>
       <c r="L28" s="5">
         <v>27</v>
       </c>
@@ -2315,7 +2274,6 @@
         <v>10</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="12"/>
       <c r="L29" s="5">
         <v>28</v>
       </c>
@@ -2350,7 +2308,6 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="12"/>
       <c r="L30" s="8">
         <v>29</v>
       </c>
@@ -2381,7 +2338,6 @@
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="12"/>
       <c r="L31" s="5">
         <v>30</v>
       </c>
@@ -2414,7 +2370,6 @@
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="12"/>
       <c r="L32" s="5">
         <v>31</v>
       </c>
@@ -2443,7 +2398,6 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="12"/>
       <c r="L33" s="5">
         <v>32</v>
       </c>
@@ -2478,7 +2432,6 @@
         <v>4</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="12"/>
       <c r="L34" s="5">
         <v>33</v>
       </c>
@@ -2515,7 +2468,6 @@
         <v>12</v>
       </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="12"/>
       <c r="L35" s="5">
         <v>34</v>
       </c>
@@ -2548,7 +2500,6 @@
         <v>5</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="12"/>
       <c r="L36" s="5">
         <v>35</v>
       </c>
@@ -2579,7 +2530,6 @@
         <v>11</v>
       </c>
       <c r="I37" s="4"/>
-      <c r="J37" s="12"/>
       <c r="L37" s="5">
         <v>36</v>
       </c>
@@ -2612,7 +2562,6 @@
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="12"/>
       <c r="L38" s="5">
         <v>37</v>
       </c>
@@ -2641,7 +2590,6 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="12"/>
       <c r="L39" s="5">
         <v>38</v>
       </c>
@@ -2674,7 +2622,7 @@
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="12" t="s">
         <v>119</v>
       </c>
       <c r="L40" s="5">
@@ -2697,7 +2645,7 @@
       <c r="A41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C41" s="4"/>
@@ -2711,7 +2659,6 @@
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="12"/>
       <c r="L41" s="5">
         <v>40</v>
       </c>
@@ -2732,7 +2679,7 @@
       <c r="A42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="16" t="s">
         <v>125</v>
       </c>
       <c r="C42" s="4"/>
@@ -2746,7 +2693,6 @@
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="12"/>
       <c r="L42" s="5">
         <v>41</v>
       </c>
@@ -2765,7 +2711,7 @@
       <c r="A43" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C43" s="4"/>
@@ -2779,7 +2725,6 @@
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="12"/>
       <c r="L43" s="5">
         <v>42</v>
       </c>
@@ -2798,7 +2743,7 @@
       <c r="A44" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="16" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="4"/>
@@ -2812,7 +2757,6 @@
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="12"/>
       <c r="L44" s="5">
         <v>43</v>
       </c>
@@ -2829,7 +2773,7 @@
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="16" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="4"/>
@@ -2848,7 +2792,7 @@
       <c r="A46" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="16" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="4"/>
@@ -2862,7 +2806,7 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="13">
+      <c r="J46" s="11">
         <v>1</v>
       </c>
       <c r="L46" s="3" t="s">
@@ -2876,7 +2820,7 @@
       <c r="A47" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="16" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="4"/>
@@ -2890,7 +2834,7 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="13">
+      <c r="J47" s="11">
         <v>1</v>
       </c>
       <c r="L47" s="3" t="s">
@@ -2904,7 +2848,7 @@
       <c r="A48" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="4"/>
@@ -2918,7 +2862,7 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="13">
+      <c r="J48" s="11">
         <v>1</v>
       </c>
       <c r="L48" s="3" t="s">
@@ -2932,7 +2876,7 @@
       <c r="A49" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="16" t="s">
         <v>94</v>
       </c>
       <c r="C49" s="4"/>
@@ -2946,7 +2890,7 @@
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="14" t="s">
+      <c r="J49" s="12" t="s">
         <v>117</v>
       </c>
       <c r="L49" s="3" t="s">
@@ -2974,7 +2918,7 @@
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="14" t="s">
+      <c r="J50" s="12" t="s">
         <v>118</v>
       </c>
       <c r="L50" s="3" t="s">
@@ -3002,7 +2946,6 @@
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="12"/>
       <c r="L51" s="4" t="s">
         <v>86</v>
       </c>
@@ -3028,7 +2971,6 @@
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="12"/>
       <c r="L52" s="3" t="s">
         <v>106</v>
       </c>
@@ -3054,7 +2996,6 @@
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="12"/>
       <c r="L53" s="3" t="s">
         <v>109</v>
       </c>
@@ -3080,7 +3021,6 @@
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="12"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="4" t="s">
@@ -3100,7 +3040,6 @@
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="12"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="4" t="s">
@@ -3120,7 +3059,6 @@
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="12"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="4" t="s">
@@ -3140,7 +3078,6 @@
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="12"/>
     </row>
     <row r="59" spans="1:13">
       <c r="B59" s="3" t="s">
@@ -3154,7 +3091,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M51" r:id="rId1"/>
+    <hyperlink ref="M51" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3163,11 +3100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3178,232 +3115,230 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="28" t="s">
         <v>129</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="15"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="15"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="20" t="s">
         <v>121</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="32" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="27"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="1048576" spans="1:1">
       <c r="A1048576" s="4" t="s">

</xml_diff>